<commit_message>
folder added and new or old will be deleted...
</commit_message>
<xml_diff>
--- a/matrix/executed/adblocking_execute.xlsx
+++ b/matrix/executed/adblocking_execute.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\matrix\executed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2903130-51E7-4A89-A624-6B9BEDC4BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D39FDF-689E-420E-8C1B-DDD27EF4A643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,10 +269,6 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -302,73 +298,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>563880</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -2715,7 +2644,7 @@
   <dimension ref="B2:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2790,29 +2719,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId3" name="Check Box 1">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>167640</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+            <control shapeId="1026" r:id="rId3" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2834,7 +2741,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId5" name="Check Box 3">
+            <control shapeId="1027" r:id="rId4" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2856,7 +2763,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId6" name="Check Box 4">
+            <control shapeId="1028" r:id="rId5" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2878,7 +2785,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId7" name="Check Box 5">
+            <control shapeId="1029" r:id="rId6" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2900,7 +2807,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId8" name="Check Box 6">
+            <control shapeId="1030" r:id="rId7" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2922,7 +2829,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId9" name="Check Box 7">
+            <control shapeId="1031" r:id="rId8" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2944,7 +2851,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId10" name="Check Box 8">
+            <control shapeId="1032" r:id="rId9" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2966,7 +2873,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId11" name="Check Box 9">
+            <control shapeId="1033" r:id="rId10" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2988,7 +2895,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId12" name="Check Box 10">
+            <control shapeId="1034" r:id="rId11" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3010,7 +2917,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId13" name="Check Box 11">
+            <control shapeId="1035" r:id="rId12" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3032,7 +2939,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId14" name="Check Box 12">
+            <control shapeId="1036" r:id="rId13" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3054,7 +2961,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId15" name="Check Box 13">
+            <control shapeId="1037" r:id="rId14" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3076,7 +2983,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId16" name="Check Box 14">
+            <control shapeId="1038" r:id="rId15" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3098,7 +3005,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId17" name="Check Box 15">
+            <control shapeId="1039" r:id="rId16" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3120,7 +3027,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId18" name="Check Box 16">
+            <control shapeId="1040" r:id="rId17" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3142,7 +3049,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId19" name="Check Box 17">
+            <control shapeId="1041" r:id="rId18" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3164,7 +3071,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId20" name="Check Box 18">
+            <control shapeId="1042" r:id="rId19" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3186,7 +3093,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId21" name="Check Box 19">
+            <control shapeId="1043" r:id="rId20" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3208,7 +3115,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId22" name="Check Box 20">
+            <control shapeId="1044" r:id="rId21" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3230,7 +3137,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId23" name="Check Box 21">
+            <control shapeId="1045" r:id="rId22" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3252,7 +3159,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId24" name="Check Box 22">
+            <control shapeId="1046" r:id="rId23" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3274,7 +3181,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId25" name="Check Box 23">
+            <control shapeId="1047" r:id="rId24" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3296,7 +3203,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId26" name="Check Box 24">
+            <control shapeId="1048" r:id="rId25" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3318,7 +3225,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId27" name="Check Box 25">
+            <control shapeId="1049" r:id="rId26" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3340,7 +3247,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId28" name="Check Box 26">
+            <control shapeId="1050" r:id="rId27" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3362,7 +3269,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId29" name="Check Box 27">
+            <control shapeId="1051" r:id="rId28" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3384,7 +3291,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId30" name="Check Box 28">
+            <control shapeId="1052" r:id="rId29" name="Check Box 28">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3406,7 +3313,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId31" name="Check Box 29">
+            <control shapeId="1053" r:id="rId30" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3428,7 +3335,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId32" name="Check Box 30">
+            <control shapeId="1054" r:id="rId31" name="Check Box 30">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3450,7 +3357,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId33" name="Check Box 31">
+            <control shapeId="1055" r:id="rId32" name="Check Box 31">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3472,7 +3379,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId34" name="Check Box 32">
+            <control shapeId="1056" r:id="rId33" name="Check Box 32">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>